<commit_message>
tạo cấu trúc bảng dữ liệu
</commit_message>
<xml_diff>
--- a/Document/Structure_Database/tables_database.xlsx
+++ b/Document/Structure_Database/tables_database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\BaitapHK6\CongNghePhanMem\ProjectSE_Appdulichao\Document\Structure_Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{31D2E1CC-3295-425A-B21C-4BD05F78494D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3D7D0C-CBCE-4DB4-899C-9D6BF986E5DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{D5ED2D6F-BEC1-47FD-B477-1FE6F0165EBB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Locations</t>
   </si>
@@ -52,13 +52,49 @@
   </si>
   <si>
     <t>rate</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>user_hoten</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>Evaluate</t>
+  </si>
+  <si>
+    <t>numberofview</t>
+  </si>
+  <si>
+    <t>comment_id</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>gender</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,6 +106,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -89,7 +132,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -97,15 +140,86 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,67 +534,132 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C20E6460-ADE5-4E25-95E6-9C35DC70664B}">
-  <dimension ref="C6:D14"/>
+  <dimension ref="C5:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="3:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
+      <c r="D6" s="2"/>
+      <c r="F6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="I6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C7" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
+      <c r="D7" s="4"/>
+      <c r="F7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="I7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C8" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
+      <c r="D8" s="4"/>
+      <c r="F8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="I8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C9" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
+      <c r="D9" s="4"/>
+      <c r="F9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="I9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C11" t="s">
+      <c r="D10" s="4"/>
+      <c r="F10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="I10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C11" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C12" t="s">
+      <c r="D11" s="4"/>
+      <c r="F11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C12" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C13" t="s">
+      <c r="D12" s="4"/>
+      <c r="F12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C14" t="s">
-        <v>8</v>
-      </c>
+      <c r="D13" s="4"/>
+      <c r="F13" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="I6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
chỉnh sửa cấu trúc dữ liệu
</commit_message>
<xml_diff>
--- a/Document/Structure_Database/tables_database.xlsx
+++ b/Document/Structure_Database/tables_database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\BaitapHK6\CongNghePhanMem\ProjectSE_Appdulichao\Document\Structure_Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3D7D0C-CBCE-4DB4-899C-9D6BF986E5DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E39943-6718-4EAE-9E9E-276791048442}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{D5ED2D6F-BEC1-47FD-B477-1FE6F0165EBB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Locations</t>
   </si>
@@ -88,6 +88,18 @@
   </si>
   <si>
     <t>gender</t>
+  </si>
+  <si>
+    <t>TypeAccess</t>
+  </si>
+  <si>
+    <t>typeaccess_id</t>
+  </si>
+  <si>
+    <t>typeaccess_name</t>
+  </si>
+  <si>
+    <t>typeaccess_img</t>
   </si>
 </sst>
 </file>
@@ -208,18 +220,18 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C20E6460-ADE5-4E25-95E6-9C35DC70664B}">
-  <dimension ref="C5:J14"/>
+  <dimension ref="C5:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,120 +558,144 @@
     <col min="4" max="4" width="11.6640625" customWidth="1"/>
     <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="3:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C6" s="1" t="s">
+    <row r="5" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="3:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="F6" s="1" t="s">
+      <c r="D6" s="8"/>
+      <c r="F6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="I6" s="1" t="s">
+      <c r="G6" s="8"/>
+      <c r="I6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C7" s="3" t="s">
+      <c r="J6" s="8"/>
+      <c r="L6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="F7" s="3" t="s">
+      <c r="D7" s="2"/>
+      <c r="F7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="I7" s="3" t="s">
+      <c r="G7" s="2"/>
+      <c r="I7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J7" s="4"/>
-    </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C8" s="5" t="s">
+      <c r="J7" s="2"/>
+      <c r="L7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="F8" s="5" t="s">
+      <c r="D8" s="2"/>
+      <c r="F8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="I8" s="3" t="s">
+      <c r="G8" s="2"/>
+      <c r="I8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="4"/>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C9" s="5" t="s">
+      <c r="J8" s="2"/>
+      <c r="L8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="F9" s="5" t="s">
+      <c r="D9" s="2"/>
+      <c r="F9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="I9" s="5" t="s">
+      <c r="G9" s="2"/>
+      <c r="I9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="4"/>
-    </row>
-    <row r="10" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="5" t="s">
+      <c r="J9" s="2"/>
+      <c r="L9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9" s="5"/>
+    </row>
+    <row r="10" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="F10" s="5" t="s">
+      <c r="D10" s="2"/>
+      <c r="F10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="I10" s="6" t="s">
+      <c r="G10" s="2"/>
+      <c r="I10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="7"/>
-    </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C11" s="5" t="s">
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="F11" s="5" t="s">
+      <c r="D11" s="2"/>
+      <c r="F11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C12" s="5" t="s">
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="F12" s="5" t="s">
+      <c r="D12" s="2"/>
+      <c r="F12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C13" s="5" t="s">
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="F13" s="8" t="s">
+      <c r="D13" s="2"/>
+      <c r="F13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="6" t="s">
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="I6:J6"/>
+    <mergeCell ref="L6:M6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>